<commit_message>
Fixed refactoring of import service
</commit_message>
<xml_diff>
--- a/HaurRanking/src/test/resources/HaurRanking.xlsx
+++ b/HaurRanking/src/test/resources/HaurRanking.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30382" windowHeight="12833" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15524" windowHeight="7121" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
     <sheet name="Taul2" sheetId="2" r:id="rId2"/>
     <sheet name="Taul3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="F32" sqref="F32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
@@ -712,7 +712,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -771,9 +773,6 @@
         <v>3.6</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="3">
-        <v>3.8</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -913,7 +912,7 @@
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="7">
-        <v>2.65</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
@@ -964,11 +963,9 @@
         <v>1.1803300000000001</v>
       </c>
       <c r="J25" s="17"/>
-      <c r="K25" s="16">
-        <v>1.4339599999999999</v>
-      </c>
+      <c r="K25" s="16"/>
       <c r="L25" s="16">
-        <v>1.2527200000000001</v>
+        <v>1.1620900000000001</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
@@ -995,7 +992,7 @@
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="16">
-        <v>0.56603999999999999</v>
+        <v>0.83333000000000002</v>
       </c>
       <c r="L26" s="16">
         <v>0.87204000000000004</v>
@@ -1024,9 +1021,11 @@
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="16"/>
+      <c r="K27" s="16">
+        <v>1.1666700000000001</v>
+      </c>
       <c r="L27" s="16">
-        <v>0.81799999999999995</v>
+        <v>1.0040100000000001</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
@@ -1084,19 +1083,20 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="4">
-        <v>0.7</v>
-      </c>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G32" s="4"/>
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="4">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Import fixed to stop from saving stages that are already in DB
</commit_message>
<xml_diff>
--- a/HaurRanking/src/test/resources/HaurRanking.xlsx
+++ b/HaurRanking/src/test/resources/HaurRanking.xlsx
@@ -33,30 +33,15 @@
     <t>CLC-01</t>
   </si>
   <si>
-    <t>CLC-02</t>
-  </si>
-  <si>
     <t>CLC-03</t>
   </si>
   <si>
-    <t>CLC-04</t>
-  </si>
-  <si>
     <t>CLC-05</t>
   </si>
   <si>
-    <t>CLC-06</t>
-  </si>
-  <si>
     <t>CLC-07</t>
   </si>
   <si>
-    <t>CLC-08</t>
-  </si>
-  <si>
-    <t>CLC-10</t>
-  </si>
-  <si>
     <t>Jarno Virta</t>
   </si>
   <si>
@@ -81,16 +66,10 @@
     <t>MATCH: "Old match" (12.11.2017)</t>
   </si>
   <si>
-    <t xml:space="preserve">CLC-09 </t>
-  </si>
-  <si>
     <t>MATCH: "Spring match" (1.4.2017)</t>
   </si>
   <si>
     <t>Jarno Virta (more than 8 results)</t>
-  </si>
-  <si>
-    <t>Jarno Virta (CLC-04 result dropped out because more than 8 results)</t>
   </si>
   <si>
     <t>Rob Leatham (not enough results)</t>
@@ -154,6 +133,27 @@
   </si>
   <si>
     <t>RANKING: PRODUCTION</t>
+  </si>
+  <si>
+    <t>CLC-09</t>
+  </si>
+  <si>
+    <t>CLC-11</t>
+  </si>
+  <si>
+    <t>CLC-13</t>
+  </si>
+  <si>
+    <t>CLC-15</t>
+  </si>
+  <si>
+    <t>CLC-17</t>
+  </si>
+  <si>
+    <t>CLC-19</t>
+  </si>
+  <si>
+    <t>Jarno Virta (CLC-07 result dropped out because more than 8 results)</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,6 +239,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -580,7 +581,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:G32"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
@@ -599,10 +600,10 @@
     </row>
     <row r="4" spans="1:11" ht="58.55" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -622,27 +623,27 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -663,10 +664,13 @@
         <v>4.5</v>
       </c>
       <c r="J6" s="10"/>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>3.1</v>
@@ -691,7 +695,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>1.5</v>
@@ -718,7 +722,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -753,12 +757,12 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -776,7 +780,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -807,12 +811,12 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="29.3" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E16" s="10">
         <v>5.0999999999999996</v>
@@ -820,7 +824,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>3.5</v>
@@ -841,7 +845,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B18" s="10">
         <v>2.2000000000000002</v>
@@ -859,7 +863,7 @@
     </row>
     <row r="19" spans="1:12" ht="43.95" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -884,7 +888,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B22" s="7">
         <v>3.55</v>
@@ -930,15 +934,15 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B25" s="16">
         <v>1.12676</v>
@@ -963,44 +967,46 @@
         <v>1.1803300000000001</v>
       </c>
       <c r="J25" s="17"/>
-      <c r="K25" s="16"/>
+      <c r="K25" s="16">
+        <v>0.55556000000000005</v>
+      </c>
       <c r="L25" s="16">
         <v>1.1620900000000001</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="16">
+        <v>7</v>
+      </c>
+      <c r="B26" s="18">
         <v>0.87324000000000002</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="16">
+      <c r="E26" s="18">
         <v>0.86667000000000005</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16">
         <v>0.73016000000000003</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="18">
         <v>0.92857000000000001</v>
       </c>
       <c r="I26" s="16">
         <v>0.81967000000000001</v>
       </c>
       <c r="J26" s="17"/>
-      <c r="K26" s="16">
+      <c r="K26" s="18">
         <v>0.83333000000000002</v>
       </c>
       <c r="L26" s="16">
-        <v>0.87204000000000004</v>
+        <v>0.87544999999999995</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B27" s="16">
         <v>0.42254000000000003</v>
@@ -1030,7 +1036,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B28" s="16">
         <v>0.56337999999999999</v>
@@ -1065,16 +1071,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
@@ -1083,7 +1089,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B32" s="4">
         <v>0.86399999999999999</v>
@@ -1093,15 +1099,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B33" s="4">
-        <v>0.75</v>
+        <v>0.75329999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4"/>
     </row>

</xml_diff>

<commit_message>
Merge and update todo
</commit_message>
<xml_diff>
--- a/HaurRanking/src/test/resources/HaurRanking.xlsx
+++ b/HaurRanking/src/test/resources/HaurRanking.xlsx
@@ -239,7 +239,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>

</xml_diff>